<commit_message>
Update sheet name to 'Chart'
</commit_message>
<xml_diff>
--- a/src/net/datenwerke/rs/samples/templates/jxls/jxlsreports/chart.xlsx
+++ b/src/net/datenwerke/rs/samples/templates/jxls/jxlsreports/chart.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NDI_customize\NDW\NDW_Migration\IA_student_Allard\JXLS\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allard/Desktop/reportserver-samples/src/net/datenwerke/rs/samples/templates/jxls/jxlsreports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3BC021-DE15-4AB4-BB4F-BDB1AC9FEB69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA6D9BE-C8D4-0746-8A4D-FA890F8AD155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-15480" windowWidth="19440" windowHeight="15000" xr2:uid="{D1D06D48-80CB-4375-B195-0904EBD3758D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{D1D06D48-80CB-4375-B195-0904EBD3758D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Multiple Queries" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -240,7 +240,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -318,7 +318,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Multiple Queries'!$C$7</c:f>
+              <c:f>Chart!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -339,7 +339,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Multiple Queries'!$A$8:$A$13</c:f>
+              <c:f>Chart!$A$8:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -359,7 +359,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Multiple Queries'!$C$8:$C$13</c:f>
+              <c:f>Chart!$C$8:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -401,7 +401,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Multiple Queries'!$B$7:$B$8</c15:sqref>
+                          <c15:sqref>Chart!$B$7:$B$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -431,7 +431,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Multiple Queries'!$A$8:$A$13</c15:sqref>
+                          <c15:sqref>Chart!$A$8:$A$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -457,7 +457,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Multiple Queries'!$B$9:$B$13</c15:sqref>
+                          <c15:sqref>Chart!$B$9:$B$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -480,10 +480,10 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Multiple Queries'!$C$7:$C$8</c15:sqref>
+                          <c15:sqref>Chart!$C$7:$C$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -510,10 +510,10 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Multiple Queries'!$A$8:$A$13</c15:sqref>
+                          <c15:sqref>Chart!$A$8:$A$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -536,10 +536,10 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Multiple Queries'!$C$9:$C$13</c15:sqref>
+                          <c15:sqref>Chart!$C$9:$C$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -552,7 +552,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-E6A4-47F7-BC2A-82BC927D7BE8}"/>
                   </c:ext>
@@ -1604,18 +1604,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C838B6D9-6BCB-41EF-9B8B-741AEE66B68F}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1642,24 +1642,24 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1681,12 +1681,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1696,22 +1696,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
modify last-tested version and notes
</commit_message>
<xml_diff>
--- a/src/net/datenwerke/rs/samples/templates/jxls/jxlsreports/chart.xlsx
+++ b/src/net/datenwerke/rs/samples/templates/jxls/jxlsreports/chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allard/Desktop/reportserver-samples/src/net/datenwerke/rs/samples/templates/jxls/jxlsreports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA6D9BE-C8D4-0746-8A4D-FA890F8AD155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047F167E-47DB-4176-99B2-BD6FD8E4F94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{D1D06D48-80CB-4375-B195-0904EBD3758D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24075" windowHeight="12885" xr2:uid="{D1D06D48-80CB-4375-B195-0904EBD3758D}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Employee Number:</t>
   </si>
@@ -132,7 +132,10 @@
     <t>(Version: 1.0.1)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Last tested with: ReportServer 4.0.0-6053) </t>
+    <t xml:space="preserve">(Last tested with: ReportServer 4.1.0-6064) </t>
+  </si>
+  <si>
+    <t>(Note that in order to create the chart, we would need to know where the chart data is going appear to select the correct cell ranges for the axes.)</t>
   </si>
 </sst>
 </file>
@@ -222,7 +225,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -240,7 +243,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -302,7 +305,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -603,7 +606,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="957054640"/>
@@ -662,7 +665,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="962381472"/>
@@ -710,7 +713,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1306,7 +1309,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1602,20 +1605,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C838B6D9-6BCB-41EF-9B8B-741AEE66B68F}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1627,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1633,7 +1636,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1642,24 +1645,24 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1681,12 +1684,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1696,24 +1699,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>